<commit_message>
Working on report, finished signalsCCC
</commit_message>
<xml_diff>
--- a/Proj2Signals.xlsx
+++ b/Proj2Signals.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+  <si>
+    <t xml:space="preserve">FETCH</t>
+  </si>
   <si>
     <t xml:space="preserve">DECODE</t>
   </si>
@@ -83,6 +86,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">PC Stall</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -181,6 +187,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">IFID Stall</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -230,6 +239,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">IFID Flush</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -379,6 +391,28 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">FWD Data        </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">CONSUMED</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">BRANCH         </t>
     </r>
     <r>
@@ -509,9 +543,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">`</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -566,6 +597,38 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
+      <t xml:space="preserve">FWD A              </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">GEN+CONSUMED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">SIGNEXT </t>
     </r>
     <r>
@@ -579,6 +642,46 @@
       </rPr>
       <t xml:space="preserve">GEN+CONSUMED</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">FWD B              </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">GEN+CONSUMED</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">IDEX Stall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXMEM Stall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEMWB Stall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDEX Flush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXMEM Flush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEMWB Flush</t>
   </si>
 </sst>
 </file>
@@ -588,7 +691,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -618,6 +721,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -688,21 +798,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.9"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,127 +826,167 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>19</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>21</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>23</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>25</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="0" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>27</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
         <v>32</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>